<commit_message>
First Results For NN Size
</commit_message>
<xml_diff>
--- a/ConvFilter Calculations..xlsx
+++ b/ConvFilter Calculations..xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/staque/Development/GitHub/CS-660-Semester-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/staque/Development/GitHub/CS-660-Semester-Project-V2/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -397,7 +397,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -442,48 +442,48 @@
         <v>5</v>
       </c>
       <c r="E2" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F2" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <f>_xlfn.FLOOR.MATH(((A2-CFilter1)/CStride1)+1)</f>
-        <v>96</v>
+        <v>238</v>
       </c>
       <c r="B3" s="1">
         <f>_xlfn.FLOOR.MATH(((B2-CFilter1)/CStride1)+1)</f>
-        <v>128</v>
+        <v>318</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E3" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <f>_xlfn.FLOOR.MATH(((A3-PFilter1)/PStride1)+1)</f>
-        <v>19</v>
+        <v>119</v>
       </c>
       <c r="B4" s="1">
         <f>_xlfn.FLOOR.MATH(((B3-PFilter1)/PStride1)+1)</f>
-        <v>25</v>
+        <v>159</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -499,21 +499,21 @@
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <f>_xlfn.FLOOR.MATH(((A4-CFilter2)/CStride2)+1)</f>
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="B5" s="1">
         <f>_xlfn.FLOOR.MATH(((B4-CFilter2)/CStride2)+1)</f>
-        <v>24</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <f>_xlfn.FLOOR.MATH(((A5-PFilter2)/PStride2)+1)</f>
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1">
         <f>_xlfn.FLOOR.MATH(((B5-PFilter2)/PStride2)+1)</f>
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>